<commit_message>
mise à jour du registre des actions
</commit_message>
<xml_diff>
--- a/Gestion de projet/Registre des actions.xlsx
+++ b/Gestion de projet/Registre des actions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Documents\SPORTIFS\sportifs.documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Documents\SPORTIFS\sportifs.documents\Gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2045,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,13 +3184,11 @@
         <v>41600</v>
       </c>
       <c r="G39" s="1">
-        <v>41607</v>
-      </c>
-      <c r="H39" s="1">
-        <v>41607</v>
-      </c>
+        <v>41618</v>
+      </c>
+      <c r="H39" s="1"/>
       <c r="I39" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>